<commit_message>
SubCalc contour updates, small FIELDS updates
</commit_message>
<xml_diff>
--- a/templates/subcalc_template.xlsx
+++ b/templates/subcalc_template.xlsx
@@ -32,18 +32,9 @@
     <t>Of Concern?</t>
   </si>
   <si>
-    <t>Tag</t>
-  </si>
-  <si>
-    <t>The SubCalc template should be filled out as a flat file with entries in all columns for all rows.</t>
-  </si>
-  <si>
     <t>Name:</t>
   </si>
   <si>
-    <t>The name or title of the footprint. Rows with identical names are assumed to be part of the same footprint.</t>
-  </si>
-  <si>
     <t>X:</t>
   </si>
   <si>
@@ -68,10 +59,19 @@
     <t>A flag indicating whether the footprint coordinates should be closed upon plotting (1 = yes, 0 = no)</t>
   </si>
   <si>
-    <t>Footprints with identical tags will be plotted/labeled as a group</t>
-  </si>
-  <si>
     <t>Group</t>
+  </si>
+  <si>
+    <t>The SubCalc template should be filled out as a flat file with entries in all columns for all rows, then saved as a csv.</t>
+  </si>
+  <si>
+    <t>Group:</t>
+  </si>
+  <si>
+    <t>Label identifiying unique footprints. This label won't be plotted.</t>
+  </si>
+  <si>
+    <t>Label identifying groups of footprints that are plotted under the same label. This label will be plotted.</t>
   </si>
 </sst>
 </file>
@@ -563,14 +563,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="43"/>
   </cellXfs>
   <cellStyles count="45">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -983,7 +982,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -994,64 +993,64 @@
   <sheetData>
     <row r="1" spans="1:2" s="3" customFormat="1">
       <c r="A1" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="3" customFormat="1"/>
     <row r="3" spans="1:2" s="3" customFormat="1">
       <c r="A3" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>10</v>
+    <row r="4" spans="1:2" s="3" customFormat="1">
+      <c r="A4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1069,16 +1068,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G42"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="4" width="9.140625" style="2"/>
-    <col min="5" max="5" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="4" width="9.140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="2"/>
@@ -1086,7 +1085,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
@@ -1104,213 +1103,8 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-    </row>
-    <row r="17" spans="2:4">
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-    </row>
-    <row r="18" spans="2:4">
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-    </row>
-    <row r="19" spans="2:4">
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-    </row>
-    <row r="20" spans="2:4">
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-    </row>
-    <row r="21" spans="2:4">
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-    </row>
-    <row r="22" spans="2:4">
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-    </row>
-    <row r="23" spans="2:4">
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-    </row>
-    <row r="24" spans="2:4">
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-    </row>
-    <row r="25" spans="2:4">
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-    </row>
-    <row r="26" spans="2:4">
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-    </row>
-    <row r="27" spans="2:4">
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-    </row>
-    <row r="28" spans="2:4">
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-    </row>
-    <row r="29" spans="2:4">
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-    </row>
-    <row r="30" spans="2:4">
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-    </row>
-    <row r="31" spans="2:4">
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-    </row>
-    <row r="32" spans="2:4">
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-    </row>
-    <row r="33" spans="2:4">
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-    </row>
-    <row r="34" spans="2:4">
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-    </row>
-    <row r="35" spans="2:4">
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-    </row>
-    <row r="36" spans="2:4">
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-    </row>
-    <row r="37" spans="2:4">
-      <c r="B37" s="4"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
-    </row>
-    <row r="38" spans="2:4">
-      <c r="B38" s="4"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
-    </row>
-    <row r="39" spans="2:4">
-      <c r="B39" s="4"/>
-      <c r="C39" s="4"/>
-      <c r="D39" s="4"/>
-    </row>
-    <row r="40" spans="2:4">
-      <c r="B40" s="4"/>
-      <c r="C40" s="4"/>
-      <c r="D40" s="4"/>
-    </row>
-    <row r="41" spans="2:4">
-      <c r="B41" s="4"/>
-      <c r="C41" s="4"/>
-      <c r="D41" s="4"/>
-    </row>
-    <row r="42" spans="2:4">
-      <c r="B42" s="4"/>
-      <c r="C42" s="4"/>
-      <c r="D42" s="4"/>
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>

</xml_diff>

<commit_message>
Modularize subcalc.plot_contours() to prepare for more plot types and add linear scale option
</commit_message>
<xml_diff>
--- a/templates/subcalc_template.xlsx
+++ b/templates/subcalc_template.xlsx
@@ -982,7 +982,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD11"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -999,18 +999,18 @@
     <row r="2" spans="1:2" s="3" customFormat="1"/>
     <row r="3" spans="1:2" s="3" customFormat="1">
       <c r="A3" s="3" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:2" s="3" customFormat="1">
       <c r="A4" s="3" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1071,7 +1071,7 @@
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1085,10 +1085,10 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>

</xml_diff>